<commit_message>
Acta de Relatorio de Proyecto
Acta de Relatorio de Proyecto
</commit_message>
<xml_diff>
--- a/Area_de_Proceso-_PP-PMC/ACREPRO/ACREPRO_DD_MM_2015.xlsx
+++ b/Area_de_Proceso-_PP-PMC/ACREPRO/ACREPRO_DD_MM_2015.xlsx
@@ -5,22 +5,23 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Perochena\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Perochena\Documents\GitHub\UTP-GPS-ALARM\Area_de_Proceso-_PP-PMC\ACREPRO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Descripción Lecciones Aprendida" sheetId="1" r:id="rId1"/>
     <sheet name="Plantilla Lecciones Aprendidas" sheetId="7" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t>#</t>
   </si>
@@ -113,6 +114,72 @@
   </si>
   <si>
     <t>Relatorio de Proyecto</t>
+  </si>
+  <si>
+    <t>UTP-GPS-ALARM</t>
+  </si>
+  <si>
+    <t>MST-EIRL</t>
+  </si>
+  <si>
+    <t>Edwar Gaspar, Julio Leonardo, Roger Apaestegui</t>
+  </si>
+  <si>
+    <t>Plan de Proyecto</t>
+  </si>
+  <si>
+    <t>No sabiamos como elaborar un plan de proyecto de software adecuado</t>
+  </si>
+  <si>
+    <t>PP-PMC</t>
+  </si>
+  <si>
+    <t>Requerimientos</t>
+  </si>
+  <si>
+    <t>Usar como guia los documentos de plan entregados por el profesor para realizarlo en el nuestro, se coordino con el profesor todo lo relacionado al plan de proyecto</t>
+  </si>
+  <si>
+    <t>Se realizo un correcto documento de Plan de Proyecto teniendo en cuenta los standares de CMMI</t>
+  </si>
+  <si>
+    <t>Revisar muy bien todos los documentos que involucran a plan de proyectos , asi como nomenclaturas y funciones de cada integrante del grupo</t>
+  </si>
+  <si>
+    <t>Metricas de Software</t>
+  </si>
+  <si>
+    <t>No se sabia como hacer la elaboracion  y uso de las metricas en el desarrollo de un software</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>Ejecucion , Seguimiento  Control</t>
+  </si>
+  <si>
+    <t>Coordinar con el profesor como hacer un correcto trabajo de metricas , formulas , y para que sirven estos datos obtenidos , establecer las acciones a corregir de acuerdo al semaforo  de resultados</t>
+  </si>
+  <si>
+    <t>Se aprendio que las metricas sirven para dar un termometro en tiempo real de los avances y procesos de un proyecto , se mide la calidad , desviaciones  de este y se hace un ajuste de acuerdo a los resultados obtenidos</t>
+  </si>
+  <si>
+    <t>Es muy importante establecer metricas y que los datos de las formulas sean precisos ya que de lo contrario las metricas se mediran mal y no se tendran resultados certeros.</t>
+  </si>
+  <si>
+    <t>Cambiar requerimientos a mitad de proyecto afectan los tiempos de trabajo</t>
+  </si>
+  <si>
+    <t>REQM</t>
+  </si>
+  <si>
+    <t>Se establecio una solicitud de cambios para fusionar dos modulos , se descarto las otras 3 "cambio de logo,pagina web" para evitar caer en desfase de tiempo de entrga de proyecto</t>
+  </si>
+  <si>
+    <t>Se aprendio que no se puede cambiar los requerimientos tan facil cuando el proyecto a esta a mitad o casi por terminar porque afecta a todos los documentos involucrados y eso amerita mas tiempo.</t>
+  </si>
+  <si>
+    <t>Es importante establecer muy bien los requerimientos del proyecto al iniciar el mismo</t>
   </si>
 </sst>
 </file>
@@ -522,7 +589,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -566,6 +633,138 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -573,123 +772,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1145,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:I7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,156 +1245,156 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="38"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
     </row>
     <row r="3" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="44"/>
     </row>
     <row r="4" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="44"/>
     </row>
     <row r="5" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="41"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="44"/>
     </row>
     <row r="6" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="42"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="44"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="47"/>
     </row>
     <row r="7" spans="2:9" ht="27" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="56"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="51"/>
     </row>
     <row r="8" spans="2:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="22"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="24"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="25"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="45" t="s">
+      <c r="C9" s="29"/>
+      <c r="D9" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="47"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="28"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="51">
+      <c r="C10" s="29"/>
+      <c r="D10" s="30">
         <v>42248</v>
       </c>
-      <c r="E10" s="46"/>
-      <c r="F10" s="52"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="38"/>
       <c r="G10" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="51">
+      <c r="H10" s="30">
         <v>42327</v>
       </c>
-      <c r="I10" s="47"/>
+      <c r="I10" s="28"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="45" t="s">
+      <c r="C11" s="29"/>
+      <c r="D11" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="47"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="28"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="45" t="s">
+      <c r="C12" s="32"/>
+      <c r="D12" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="47"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="28"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="48" t="s">
+      <c r="C13" s="34"/>
+      <c r="D13" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="50"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="37"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="45" t="s">
+      <c r="C14" s="29"/>
+      <c r="D14" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="47"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="28"/>
     </row>
     <row r="15" spans="2:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="21"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="22"/>
     </row>
     <row r="16" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
@@ -1366,101 +1448,159 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="3"/>
+    <row r="18" spans="2:9" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="15">
+        <v>1</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="153" x14ac:dyDescent="0.25">
+      <c r="B19" s="15">
+        <v>1</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="15">
+        <v>1</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="3"/>
+      <c r="B21" s="15">
+        <v>1</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="17"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="3"/>
+      <c r="B22" s="15">
+        <v>1</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="17"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="3"/>
+      <c r="B23" s="15">
+        <v>1</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="17"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="3"/>
+      <c r="B24" s="15">
+        <v>1</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="17"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="3"/>
+      <c r="B25" s="15">
+        <v>1</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="17"/>
     </row>
     <row r="26" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="4"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="6"/>
+      <c r="B26" s="15">
+        <v>1</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="19"/>
     </row>
     <row r="27" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D13:I13"/>
-    <mergeCell ref="D10:F10"/>
     <mergeCell ref="B2:E6"/>
     <mergeCell ref="B7:I7"/>
     <mergeCell ref="B9:C9"/>
@@ -1476,6 +1616,8 @@
     <mergeCell ref="D12:I12"/>
     <mergeCell ref="D14:I14"/>
     <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:I13"/>
+    <mergeCell ref="D10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -1487,8 +1629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,154 +1647,166 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="38"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="44"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="44"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="41"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="44"/>
     </row>
     <row r="6" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="42"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="44"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="47"/>
     </row>
     <row r="7" spans="2:9" ht="21.75" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="17"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="61"/>
     </row>
     <row r="8" spans="2:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="22"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="24"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="25"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="27"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="54"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="35"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="58"/>
       <c r="G10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="25"/>
-      <c r="I10" s="27"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="54"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="27"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="54"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="27"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="54"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="57"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="57"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="27"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="54"/>
     </row>
     <row r="16" spans="2:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="21"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="22"/>
     </row>
     <row r="17" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
@@ -1793,15 +1947,15 @@
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:I11"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:I15"/>
+    <mergeCell ref="B16:I16"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:I12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:I13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:I14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:I15"/>
-    <mergeCell ref="B16:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>